<commit_message>
current updates Laptop, 20160806
</commit_message>
<xml_diff>
--- a/MATLAB/Eingebunden/20160701_gemittelt_zusammengefasst.xlsx
+++ b/MATLAB/Eingebunden/20160701_gemittelt_zusammengefasst.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="48">
   <si>
     <t>Zeit</t>
   </si>
@@ -156,6 +157,18 @@
   </si>
   <si>
     <t>06.07.2016, 15:13:36,486</t>
+  </si>
+  <si>
+    <t>FOL</t>
+  </si>
+  <si>
+    <t>ZUL</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -509,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2082,4 +2095,1925 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:W219"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C196" workbookViewId="0">
+      <selection activeCell="P208" sqref="P208"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>15.780999999999997</v>
+      </c>
+      <c r="E2">
+        <v>20.899499999999996</v>
+      </c>
+      <c r="F2">
+        <v>19.322999999999997</v>
+      </c>
+      <c r="G2">
+        <v>19.092999999999996</v>
+      </c>
+      <c r="H2">
+        <v>19.421000000000006</v>
+      </c>
+      <c r="I2">
+        <v>19.536500000000004</v>
+      </c>
+      <c r="J2">
+        <v>18.442500000000003</v>
+      </c>
+      <c r="K2">
+        <v>16.997000000000003</v>
+      </c>
+      <c r="L2">
+        <v>17.454499999999999</v>
+      </c>
+      <c r="M2">
+        <v>17.481999999999996</v>
+      </c>
+      <c r="N2">
+        <v>17.957000000000001</v>
+      </c>
+      <c r="O2">
+        <v>16.222999999999999</v>
+      </c>
+      <c r="P2">
+        <v>19.271999999999998</v>
+      </c>
+      <c r="Q2">
+        <v>17.414999999999999</v>
+      </c>
+      <c r="R2">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="S2">
+        <v>2.5069499999999998</v>
+      </c>
+      <c r="T2">
+        <v>2.4039999999999999</v>
+      </c>
+      <c r="U2">
+        <v>2.6758499999999996</v>
+      </c>
+      <c r="V2">
+        <v>2.5365499999999996</v>
+      </c>
+      <c r="W2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>11.351499999999998</v>
+      </c>
+      <c r="E3">
+        <v>20.789499999999997</v>
+      </c>
+      <c r="F3">
+        <v>17.863499999999998</v>
+      </c>
+      <c r="G3">
+        <v>17.4435</v>
+      </c>
+      <c r="H3">
+        <v>18.138999999999999</v>
+      </c>
+      <c r="I3">
+        <v>18.278999999999996</v>
+      </c>
+      <c r="J3">
+        <v>16.314500000000002</v>
+      </c>
+      <c r="K3">
+        <v>13.5785</v>
+      </c>
+      <c r="L3">
+        <v>14.568999999999999</v>
+      </c>
+      <c r="M3">
+        <v>14.564999999999998</v>
+      </c>
+      <c r="N3">
+        <v>15.456499999999997</v>
+      </c>
+      <c r="O3">
+        <v>12.2075</v>
+      </c>
+      <c r="P3">
+        <v>17.872</v>
+      </c>
+      <c r="Q3">
+        <v>14.504000000000001</v>
+      </c>
+      <c r="R3">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="S3">
+        <v>2.4624999999999995</v>
+      </c>
+      <c r="T3">
+        <v>2.3558499999999993</v>
+      </c>
+      <c r="U3">
+        <v>2.8487999999999998</v>
+      </c>
+      <c r="V3">
+        <v>2.5624500000000001</v>
+      </c>
+      <c r="W3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>20.106500000000004</v>
+      </c>
+      <c r="E4">
+        <v>21.011499999999995</v>
+      </c>
+      <c r="F4">
+        <v>20.707000000000004</v>
+      </c>
+      <c r="G4">
+        <v>20.631999999999998</v>
+      </c>
+      <c r="H4">
+        <v>20.588500000000003</v>
+      </c>
+      <c r="I4">
+        <v>20.752499999999994</v>
+      </c>
+      <c r="J4">
+        <v>20.469500000000004</v>
+      </c>
+      <c r="K4">
+        <v>20.311</v>
+      </c>
+      <c r="L4">
+        <v>20.191499999999998</v>
+      </c>
+      <c r="M4">
+        <v>20.342000000000006</v>
+      </c>
+      <c r="N4">
+        <v>20.433999999999997</v>
+      </c>
+      <c r="O4">
+        <v>20.137999999999998</v>
+      </c>
+      <c r="P4">
+        <v>20.631999999999994</v>
+      </c>
+      <c r="Q4">
+        <v>20.271499999999996</v>
+      </c>
+      <c r="R4">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="S4">
+        <v>2.5217499999999999</v>
+      </c>
+      <c r="T4">
+        <v>2.5346499999999996</v>
+      </c>
+      <c r="U4">
+        <v>2.59545</v>
+      </c>
+      <c r="V4">
+        <v>2.5725000000000007</v>
+      </c>
+      <c r="W4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>15.824761904761907</v>
+      </c>
+      <c r="E5">
+        <v>20.891428571428566</v>
+      </c>
+      <c r="F5">
+        <v>19.323333333333331</v>
+      </c>
+      <c r="G5">
+        <v>19.10047619047619</v>
+      </c>
+      <c r="H5">
+        <v>19.435238095238098</v>
+      </c>
+      <c r="I5">
+        <v>19.564285714285717</v>
+      </c>
+      <c r="J5">
+        <v>18.474285714285713</v>
+      </c>
+      <c r="K5">
+        <v>17.042380952380956</v>
+      </c>
+      <c r="L5">
+        <v>17.494285714285713</v>
+      </c>
+      <c r="M5">
+        <v>17.524761904761903</v>
+      </c>
+      <c r="N5">
+        <v>18.000952380952384</v>
+      </c>
+      <c r="O5">
+        <v>16.268095238095242</v>
+      </c>
+      <c r="P5">
+        <v>19.335714285714282</v>
+      </c>
+      <c r="Q5">
+        <v>17.485714285714288</v>
+      </c>
+      <c r="R5">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="S5">
+        <v>1.9094285714285717</v>
+      </c>
+      <c r="T5">
+        <v>2.1161428571428571</v>
+      </c>
+      <c r="U5">
+        <v>2.4573809523809524</v>
+      </c>
+      <c r="V5">
+        <v>2.5575238095238095</v>
+      </c>
+      <c r="W5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>15.838571428571429</v>
+      </c>
+      <c r="E6">
+        <v>20.958095238095233</v>
+      </c>
+      <c r="F6">
+        <v>19.359047619047619</v>
+      </c>
+      <c r="G6">
+        <v>19.134285714285713</v>
+      </c>
+      <c r="H6">
+        <v>19.500000000000004</v>
+      </c>
+      <c r="I6">
+        <v>19.623333333333338</v>
+      </c>
+      <c r="J6">
+        <v>18.526190476190475</v>
+      </c>
+      <c r="K6">
+        <v>17.067142857142859</v>
+      </c>
+      <c r="L6">
+        <v>17.540000000000003</v>
+      </c>
+      <c r="M6">
+        <v>17.571428571428569</v>
+      </c>
+      <c r="N6">
+        <v>18.067142857142855</v>
+      </c>
+      <c r="O6">
+        <v>16.294285714285714</v>
+      </c>
+      <c r="P6">
+        <v>19.389523809523805</v>
+      </c>
+      <c r="Q6">
+        <v>17.521904761904764</v>
+      </c>
+      <c r="R6">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="S6">
+        <v>3.1882380952380953</v>
+      </c>
+      <c r="T6">
+        <v>2.7884285714285708</v>
+      </c>
+      <c r="U6">
+        <v>3.0416666666666665</v>
+      </c>
+      <c r="V6">
+        <v>2.6770952380952378</v>
+      </c>
+      <c r="W6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>16.380833333333332</v>
+      </c>
+      <c r="E7">
+        <v>20.83124999999999</v>
+      </c>
+      <c r="F7">
+        <v>20.052916666666668</v>
+      </c>
+      <c r="G7">
+        <v>20.156250000000004</v>
+      </c>
+      <c r="H7">
+        <v>19.842083333333335</v>
+      </c>
+      <c r="I7">
+        <v>19.957083333333326</v>
+      </c>
+      <c r="J7">
+        <v>19.100833333333334</v>
+      </c>
+      <c r="K7">
+        <v>17.282916666666676</v>
+      </c>
+      <c r="L7">
+        <v>17.416666666666671</v>
+      </c>
+      <c r="M7">
+        <v>17.39083333333333</v>
+      </c>
+      <c r="N7">
+        <v>17.882916666666663</v>
+      </c>
+      <c r="O7">
+        <v>16.76583333333333</v>
+      </c>
+      <c r="P7">
+        <v>20.00375</v>
+      </c>
+      <c r="Q7">
+        <v>17.672083333333337</v>
+      </c>
+      <c r="R7">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="S7">
+        <v>2.4060000000000006</v>
+      </c>
+      <c r="T7">
+        <v>2.4272083333333327</v>
+      </c>
+      <c r="U7">
+        <v>2.5726666666666667</v>
+      </c>
+      <c r="V7">
+        <v>2.5639166666666666</v>
+      </c>
+      <c r="W7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>16.38</v>
+      </c>
+      <c r="E8">
+        <v>20.83428571</v>
+      </c>
+      <c r="F8">
+        <v>20.077619049999999</v>
+      </c>
+      <c r="G8">
+        <v>20.170476189999999</v>
+      </c>
+      <c r="H8">
+        <v>19.837619050000001</v>
+      </c>
+      <c r="I8">
+        <v>19.94714286</v>
+      </c>
+      <c r="J8">
+        <v>19.085714289999999</v>
+      </c>
+      <c r="K8">
+        <v>17.286190479999998</v>
+      </c>
+      <c r="L8">
+        <v>17.47380952</v>
+      </c>
+      <c r="M8">
+        <v>17.405714289999999</v>
+      </c>
+      <c r="N8">
+        <v>17.862380949999999</v>
+      </c>
+      <c r="O8">
+        <v>16.803809520000001</v>
+      </c>
+      <c r="P8">
+        <v>20.019523809999999</v>
+      </c>
+      <c r="Q8">
+        <v>17.676190479999999</v>
+      </c>
+      <c r="R8">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="S8">
+        <v>1.8140000000000001</v>
+      </c>
+      <c r="T8">
+        <v>2.2142857139999998</v>
+      </c>
+      <c r="U8">
+        <v>2.2696666670000001</v>
+      </c>
+      <c r="V8">
+        <v>2.5917142860000002</v>
+      </c>
+      <c r="W8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>16.340000000000003</v>
+      </c>
+      <c r="E9">
+        <v>20.508095238095237</v>
+      </c>
+      <c r="F9">
+        <v>19.810952380952376</v>
+      </c>
+      <c r="G9">
+        <v>19.886190476190471</v>
+      </c>
+      <c r="H9">
+        <v>19.664761904761903</v>
+      </c>
+      <c r="I9">
+        <v>19.725238095238097</v>
+      </c>
+      <c r="J9">
+        <v>18.908095238095239</v>
+      </c>
+      <c r="K9">
+        <v>17.222857142857141</v>
+      </c>
+      <c r="L9">
+        <v>17.433333333333334</v>
+      </c>
+      <c r="M9">
+        <v>17.360476190476192</v>
+      </c>
+      <c r="N9">
+        <v>17.779523809523813</v>
+      </c>
+      <c r="O9">
+        <v>16.758571428571425</v>
+      </c>
+      <c r="P9">
+        <v>19.844761904761899</v>
+      </c>
+      <c r="Q9">
+        <v>17.635238095238094</v>
+      </c>
+      <c r="R9">
+        <v>4.9650000000000016</v>
+      </c>
+      <c r="S9">
+        <v>1.821285714285714</v>
+      </c>
+      <c r="T9">
+        <v>2.7071904761904766</v>
+      </c>
+      <c r="U9">
+        <v>2.6066190476190472</v>
+      </c>
+      <c r="V9">
+        <v>3.371285714285714</v>
+      </c>
+      <c r="W9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>15.817</v>
+      </c>
+      <c r="E10">
+        <v>20.546500000000002</v>
+      </c>
+      <c r="F10">
+        <v>19.111000000000001</v>
+      </c>
+      <c r="G10">
+        <v>18.872</v>
+      </c>
+      <c r="H10">
+        <v>19.2575</v>
+      </c>
+      <c r="I10">
+        <v>19.283999999999999</v>
+      </c>
+      <c r="J10">
+        <v>18.281500000000001</v>
+      </c>
+      <c r="K10">
+        <v>16.984000000000002</v>
+      </c>
+      <c r="L10">
+        <v>17.471</v>
+      </c>
+      <c r="M10">
+        <v>17.4435</v>
+      </c>
+      <c r="N10">
+        <v>17.8705</v>
+      </c>
+      <c r="O10">
+        <v>16.271999999999998</v>
+      </c>
+      <c r="P10">
+        <v>19.177499999999998</v>
+      </c>
+      <c r="Q10">
+        <v>17.4345</v>
+      </c>
+      <c r="R10">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="S10">
+        <v>1.8867499999999999</v>
+      </c>
+      <c r="T10">
+        <v>2.4314</v>
+      </c>
+      <c r="U10">
+        <v>2.84815</v>
+      </c>
+      <c r="V10">
+        <v>3.2801999999999998</v>
+      </c>
+      <c r="W10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>29.31</v>
+      </c>
+      <c r="E11">
+        <v>20.864761900000001</v>
+      </c>
+      <c r="F11">
+        <v>23.318571429999999</v>
+      </c>
+      <c r="G11">
+        <v>23.63047619</v>
+      </c>
+      <c r="H11">
+        <v>23.228571429999999</v>
+      </c>
+      <c r="I11">
+        <v>23.225714289999999</v>
+      </c>
+      <c r="J11">
+        <v>24.766190479999999</v>
+      </c>
+      <c r="K11">
+        <v>27.277142860000001</v>
+      </c>
+      <c r="L11">
+        <v>26.342380949999999</v>
+      </c>
+      <c r="M11">
+        <v>26.631428570000001</v>
+      </c>
+      <c r="N11">
+        <v>25.660952380000001</v>
+      </c>
+      <c r="O11">
+        <v>28.394761899999999</v>
+      </c>
+      <c r="P11">
+        <v>23.292380949999998</v>
+      </c>
+      <c r="Q11">
+        <v>26.353809519999999</v>
+      </c>
+      <c r="R11">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="S11">
+        <v>1.876809524</v>
+      </c>
+      <c r="T11">
+        <v>2.5532380950000002</v>
+      </c>
+      <c r="U11">
+        <v>2.3253809520000002</v>
+      </c>
+      <c r="V11">
+        <v>3.2585714289999999</v>
+      </c>
+      <c r="W11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12">
+        <v>-8.5766666669999996</v>
+      </c>
+      <c r="E12">
+        <v>20.492857140000002</v>
+      </c>
+      <c r="F12">
+        <v>11.60714286</v>
+      </c>
+      <c r="G12">
+        <v>9.6828571429999997</v>
+      </c>
+      <c r="H12">
+        <v>7.8709523810000004</v>
+      </c>
+      <c r="I12">
+        <v>11.400476189999999</v>
+      </c>
+      <c r="J12">
+        <v>6.6985714290000002</v>
+      </c>
+      <c r="K12">
+        <v>-1.3438095240000001</v>
+      </c>
+      <c r="L12">
+        <v>-1.2152380949999999</v>
+      </c>
+      <c r="M12">
+        <v>1.11952381</v>
+      </c>
+      <c r="N12">
+        <v>5.5685714290000004</v>
+      </c>
+      <c r="O12">
+        <v>-5.3571428570000004</v>
+      </c>
+      <c r="P12">
+        <v>11.073809519999999</v>
+      </c>
+      <c r="Q12">
+        <v>0.97714285700000003</v>
+      </c>
+      <c r="R12">
+        <v>4.9669999999999996</v>
+      </c>
+      <c r="S12">
+        <v>3.0947619049999999</v>
+      </c>
+      <c r="T12">
+        <v>1.5409999999999999</v>
+      </c>
+      <c r="U12">
+        <v>2.2884761899999999</v>
+      </c>
+      <c r="V12">
+        <v>1.3169523809999999</v>
+      </c>
+      <c r="W12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13">
+        <v>-8.6142857142857139</v>
+      </c>
+      <c r="E13">
+        <v>20.444285714285712</v>
+      </c>
+      <c r="F13">
+        <v>11.606666666666667</v>
+      </c>
+      <c r="G13">
+        <v>9.637142857142857</v>
+      </c>
+      <c r="H13">
+        <v>7.706190476190474</v>
+      </c>
+      <c r="I13">
+        <v>11.39190476190476</v>
+      </c>
+      <c r="J13">
+        <v>6.6380952380952385</v>
+      </c>
+      <c r="K13">
+        <v>-1.3600000000000003</v>
+      </c>
+      <c r="L13">
+        <v>-1.2233333333333336</v>
+      </c>
+      <c r="M13">
+        <v>1.136190476190476</v>
+      </c>
+      <c r="N13">
+        <v>5.5514285714285725</v>
+      </c>
+      <c r="O13">
+        <v>-5.3314285714285701</v>
+      </c>
+      <c r="P13">
+        <v>11.040476190476191</v>
+      </c>
+      <c r="Q13">
+        <v>0.97714285714285731</v>
+      </c>
+      <c r="R13">
+        <v>4.9669999999999996</v>
+      </c>
+      <c r="S13">
+        <v>3.0865238095238099</v>
+      </c>
+      <c r="T13">
+        <v>1.7492857142857143</v>
+      </c>
+      <c r="U13">
+        <v>2.8587142857142855</v>
+      </c>
+      <c r="V13">
+        <v>1.6121428571428573</v>
+      </c>
+      <c r="W13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>-8.6399999999999988</v>
+      </c>
+      <c r="E14">
+        <v>20.41954545454546</v>
+      </c>
+      <c r="F14">
+        <v>11.613636363636365</v>
+      </c>
+      <c r="G14">
+        <v>9.5968181818181844</v>
+      </c>
+      <c r="H14">
+        <v>7.7077272727272739</v>
+      </c>
+      <c r="I14">
+        <v>11.434090909090909</v>
+      </c>
+      <c r="J14">
+        <v>6.6563636363636363</v>
+      </c>
+      <c r="K14">
+        <v>-1.3163636363636362</v>
+      </c>
+      <c r="L14">
+        <v>-1.1077272727272727</v>
+      </c>
+      <c r="M14">
+        <v>1.2268181818181818</v>
+      </c>
+      <c r="N14">
+        <v>5.622272727272728</v>
+      </c>
+      <c r="O14">
+        <v>-5.3599999999999994</v>
+      </c>
+      <c r="P14">
+        <v>11.085000000000001</v>
+      </c>
+      <c r="Q14">
+        <v>1.0259090909090909</v>
+      </c>
+      <c r="R14">
+        <v>4.9664545454545435</v>
+      </c>
+      <c r="S14">
+        <v>3.0643636363636362</v>
+      </c>
+      <c r="T14">
+        <v>2.0231363636363637</v>
+      </c>
+      <c r="U14">
+        <v>3.4070000000000005</v>
+      </c>
+      <c r="V14">
+        <v>1.9441363636363638</v>
+      </c>
+      <c r="W14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15">
+        <v>-8.5990476190000003</v>
+      </c>
+      <c r="E15">
+        <v>20.40095238</v>
+      </c>
+      <c r="F15">
+        <v>11.67857143</v>
+      </c>
+      <c r="G15">
+        <v>9.65</v>
+      </c>
+      <c r="H15">
+        <v>7.947619048</v>
+      </c>
+      <c r="I15">
+        <v>11.51142857</v>
+      </c>
+      <c r="J15">
+        <v>6.8490476190000003</v>
+      </c>
+      <c r="K15">
+        <v>-1.03</v>
+      </c>
+      <c r="L15">
+        <v>-0.552857143</v>
+      </c>
+      <c r="M15">
+        <v>1.6723809519999999</v>
+      </c>
+      <c r="N15">
+        <v>5.9166666670000003</v>
+      </c>
+      <c r="O15">
+        <v>-5.208571429</v>
+      </c>
+      <c r="P15">
+        <v>11.212857140000001</v>
+      </c>
+      <c r="Q15">
+        <v>1.3461904760000001</v>
+      </c>
+      <c r="R15">
+        <v>4.9660000000000002</v>
+      </c>
+      <c r="S15">
+        <v>3.0621904760000001</v>
+      </c>
+      <c r="T15">
+        <v>2.3866666670000001</v>
+      </c>
+      <c r="U15">
+        <v>3.7360000000000002</v>
+      </c>
+      <c r="V15">
+        <v>2.2970476190000002</v>
+      </c>
+      <c r="W15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16">
+        <v>-8.2885000000000026</v>
+      </c>
+      <c r="E16">
+        <v>20.211000000000002</v>
+      </c>
+      <c r="F16">
+        <v>11.756500000000001</v>
+      </c>
+      <c r="G16">
+        <v>9.6725000000000012</v>
+      </c>
+      <c r="H16">
+        <v>8.1170000000000009</v>
+      </c>
+      <c r="I16">
+        <v>11.197999999999999</v>
+      </c>
+      <c r="J16">
+        <v>7.1509999999999989</v>
+      </c>
+      <c r="K16">
+        <v>-1.0565000000000002</v>
+      </c>
+      <c r="L16">
+        <v>-0.20900000000000002</v>
+      </c>
+      <c r="M16">
+        <v>1.7284999999999999</v>
+      </c>
+      <c r="N16">
+        <v>6.2620000000000005</v>
+      </c>
+      <c r="O16">
+        <v>-4.5904999999999996</v>
+      </c>
+      <c r="P16">
+        <v>11.339</v>
+      </c>
+      <c r="Q16">
+        <v>1.6659999999999997</v>
+      </c>
+      <c r="R16">
+        <v>4.9659999999999984</v>
+      </c>
+      <c r="S16">
+        <v>3.0940000000000003</v>
+      </c>
+      <c r="T16">
+        <v>2.8208000000000006</v>
+      </c>
+      <c r="U16">
+        <v>3.8992000000000004</v>
+      </c>
+      <c r="V16">
+        <v>2.64235</v>
+      </c>
+      <c r="W16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17">
+        <v>2.1465000000000001</v>
+      </c>
+      <c r="E17">
+        <v>20.3735</v>
+      </c>
+      <c r="F17">
+        <v>15.054500000000001</v>
+      </c>
+      <c r="G17">
+        <v>13.852499999999999</v>
+      </c>
+      <c r="H17">
+        <v>13.666499999999999</v>
+      </c>
+      <c r="I17">
+        <v>14.2835</v>
+      </c>
+      <c r="J17">
+        <v>11.756500000000001</v>
+      </c>
+      <c r="K17">
+        <v>6.4909999999999997</v>
+      </c>
+      <c r="L17">
+        <v>6.8460000000000001</v>
+      </c>
+      <c r="M17">
+        <v>6.6375000000000002</v>
+      </c>
+      <c r="N17">
+        <v>9.7609999999999992</v>
+      </c>
+      <c r="O17">
+        <v>3.9445000000000001</v>
+      </c>
+      <c r="P17">
+        <v>14.7455</v>
+      </c>
+      <c r="Q17">
+        <v>7.9989999999999997</v>
+      </c>
+      <c r="R17">
+        <v>4.9660000000000002</v>
+      </c>
+      <c r="S17">
+        <v>3.0034000000000001</v>
+      </c>
+      <c r="T17">
+        <v>2.9415</v>
+      </c>
+      <c r="U17">
+        <v>3.8300999999999998</v>
+      </c>
+      <c r="V17">
+        <v>2.9885999999999999</v>
+      </c>
+      <c r="W17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>2.1970000000000001</v>
+      </c>
+      <c r="E18">
+        <v>20.387499999999999</v>
+      </c>
+      <c r="F18">
+        <v>15.031499999999999</v>
+      </c>
+      <c r="G18">
+        <v>13.843500000000001</v>
+      </c>
+      <c r="H18">
+        <v>13.513</v>
+      </c>
+      <c r="I18">
+        <v>14.029</v>
+      </c>
+      <c r="J18">
+        <v>11.691000000000001</v>
+      </c>
+      <c r="K18">
+        <v>6.3739999999999997</v>
+      </c>
+      <c r="L18">
+        <v>6.3140000000000001</v>
+      </c>
+      <c r="M18">
+        <v>6.1609999999999996</v>
+      </c>
+      <c r="N18">
+        <v>9.7025000000000006</v>
+      </c>
+      <c r="O18">
+        <v>3.8450000000000002</v>
+      </c>
+      <c r="P18">
+        <v>14.6935</v>
+      </c>
+      <c r="Q18">
+        <v>7.7945000000000002</v>
+      </c>
+      <c r="R18">
+        <v>4.9660000000000002</v>
+      </c>
+      <c r="S18">
+        <v>3.0386500000000001</v>
+      </c>
+      <c r="T18">
+        <v>2.5968</v>
+      </c>
+      <c r="U18">
+        <v>3.7002000000000002</v>
+      </c>
+      <c r="V18">
+        <v>2.6191499999999999</v>
+      </c>
+      <c r="W18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19">
+        <v>2.2324999999999999</v>
+      </c>
+      <c r="E19">
+        <v>20.371500000000001</v>
+      </c>
+      <c r="F19">
+        <v>15.164999999999999</v>
+      </c>
+      <c r="G19">
+        <v>13.922000000000001</v>
+      </c>
+      <c r="H19">
+        <v>14.038500000000001</v>
+      </c>
+      <c r="I19">
+        <v>14.467499999999999</v>
+      </c>
+      <c r="J19">
+        <v>12.087</v>
+      </c>
+      <c r="K19">
+        <v>6.7385000000000002</v>
+      </c>
+      <c r="L19">
+        <v>7.0650000000000004</v>
+      </c>
+      <c r="M19">
+        <v>7.0039999999999996</v>
+      </c>
+      <c r="N19">
+        <v>10.4245</v>
+      </c>
+      <c r="O19">
+        <v>4.2510000000000003</v>
+      </c>
+      <c r="P19">
+        <v>14.91</v>
+      </c>
+      <c r="Q19">
+        <v>8.2684999999999995</v>
+      </c>
+      <c r="R19">
+        <v>4.9659500000000003</v>
+      </c>
+      <c r="S19">
+        <v>3.0455999999999999</v>
+      </c>
+      <c r="T19">
+        <v>2.8639999999999999</v>
+      </c>
+      <c r="U19">
+        <v>3.8204500000000001</v>
+      </c>
+      <c r="V19">
+        <v>2.9841500000000001</v>
+      </c>
+      <c r="W19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E20">
+        <v>20.550999999999998</v>
+      </c>
+      <c r="F20">
+        <v>15.1265</v>
+      </c>
+      <c r="G20">
+        <v>13.96</v>
+      </c>
+      <c r="H20">
+        <v>13.826499999999999</v>
+      </c>
+      <c r="I20">
+        <v>14.3575</v>
+      </c>
+      <c r="J20">
+        <v>11.778499999999999</v>
+      </c>
+      <c r="K20">
+        <v>6.5025000000000004</v>
+      </c>
+      <c r="L20">
+        <v>6.109</v>
+      </c>
+      <c r="M20">
+        <v>6.2765000000000004</v>
+      </c>
+      <c r="N20">
+        <v>9.9425000000000008</v>
+      </c>
+      <c r="O20">
+        <v>4.0795000000000003</v>
+      </c>
+      <c r="P20">
+        <v>14.801500000000001</v>
+      </c>
+      <c r="Q20">
+        <v>7.899</v>
+      </c>
+      <c r="R20">
+        <v>4.9659000000000004</v>
+      </c>
+      <c r="S20">
+        <v>3.05585</v>
+      </c>
+      <c r="T20">
+        <v>2.3123999999999998</v>
+      </c>
+      <c r="U20">
+        <v>3.3929</v>
+      </c>
+      <c r="V20">
+        <v>2.2803499999999999</v>
+      </c>
+      <c r="W20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21">
+        <v>10.97</v>
+      </c>
+      <c r="E21">
+        <v>20.798095239999999</v>
+      </c>
+      <c r="F21">
+        <v>17.91571429</v>
+      </c>
+      <c r="G21">
+        <v>17.333333329999999</v>
+      </c>
+      <c r="H21">
+        <v>16.989047620000001</v>
+      </c>
+      <c r="I21">
+        <v>17.708571429999999</v>
+      </c>
+      <c r="J21">
+        <v>16</v>
+      </c>
+      <c r="K21">
+        <v>13.25571429</v>
+      </c>
+      <c r="L21">
+        <v>12.728571430000001</v>
+      </c>
+      <c r="M21">
+        <v>12.76857143</v>
+      </c>
+      <c r="N21">
+        <v>15.016666669999999</v>
+      </c>
+      <c r="O21">
+        <v>11.926666669999999</v>
+      </c>
+      <c r="P21">
+        <v>17.73285714</v>
+      </c>
+      <c r="Q21">
+        <v>13.83333333</v>
+      </c>
+      <c r="R21">
+        <v>4.9654761900000004</v>
+      </c>
+      <c r="S21">
+        <v>3.1681904759999999</v>
+      </c>
+      <c r="T21">
+        <v>2.4644761900000001</v>
+      </c>
+      <c r="U21">
+        <v>2.98147619</v>
+      </c>
+      <c r="V21">
+        <v>2.2579047619999999</v>
+      </c>
+      <c r="W21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22">
+        <v>11.1645</v>
+      </c>
+      <c r="E22">
+        <v>20.6645</v>
+      </c>
+      <c r="F22">
+        <v>17.8965</v>
+      </c>
+      <c r="G22">
+        <v>17.334499999999998</v>
+      </c>
+      <c r="H22">
+        <v>17.599499999999999</v>
+      </c>
+      <c r="I22">
+        <v>18.086500000000001</v>
+      </c>
+      <c r="J22">
+        <v>16.208500000000001</v>
+      </c>
+      <c r="K22">
+        <v>13.515000000000001</v>
+      </c>
+      <c r="L22">
+        <v>14.098000000000001</v>
+      </c>
+      <c r="M22">
+        <v>14.1485</v>
+      </c>
+      <c r="N22">
+        <v>15.339499999999999</v>
+      </c>
+      <c r="O22">
+        <v>12.166499999999999</v>
+      </c>
+      <c r="P22">
+        <v>17.890499999999999</v>
+      </c>
+      <c r="Q22">
+        <v>14.2675</v>
+      </c>
+      <c r="R22">
+        <v>4.9650499999999997</v>
+      </c>
+      <c r="S22">
+        <v>3.1676000000000002</v>
+      </c>
+      <c r="T22">
+        <v>3.0297999999999998</v>
+      </c>
+      <c r="U22">
+        <v>3.5918000000000001</v>
+      </c>
+      <c r="V22">
+        <v>3.2702</v>
+      </c>
+      <c r="W22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23">
+        <v>11.164999999999999</v>
+      </c>
+      <c r="E23">
+        <v>20.526250000000001</v>
+      </c>
+      <c r="F23">
+        <v>17.78</v>
+      </c>
+      <c r="G23">
+        <v>17.223749999999999</v>
+      </c>
+      <c r="H23">
+        <v>17.56625</v>
+      </c>
+      <c r="I23">
+        <v>17.994999999999997</v>
+      </c>
+      <c r="J23">
+        <v>16.09</v>
+      </c>
+      <c r="K23">
+        <v>13.465000000000002</v>
+      </c>
+      <c r="L23">
+        <v>14.1275</v>
+      </c>
+      <c r="M23">
+        <v>14.1325</v>
+      </c>
+      <c r="N23">
+        <v>15.228750000000002</v>
+      </c>
+      <c r="O23">
+        <v>12.149999999999999</v>
+      </c>
+      <c r="P23">
+        <v>17.778749999999999</v>
+      </c>
+      <c r="Q23">
+        <v>14.216249999999999</v>
+      </c>
+      <c r="R23">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="S23">
+        <v>3.139875</v>
+      </c>
+      <c r="T23">
+        <v>3.0493750000000004</v>
+      </c>
+      <c r="U23">
+        <v>3.6048749999999998</v>
+      </c>
+      <c r="V23">
+        <v>3.3040000000000003</v>
+      </c>
+      <c r="W23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24">
+        <v>19.988499999999998</v>
+      </c>
+      <c r="E24">
+        <v>20.778500000000001</v>
+      </c>
+      <c r="F24">
+        <v>20.477499999999999</v>
+      </c>
+      <c r="G24">
+        <v>20.405999999999999</v>
+      </c>
+      <c r="H24">
+        <v>20.224</v>
+      </c>
+      <c r="I24">
+        <v>20.513999999999999</v>
+      </c>
+      <c r="J24">
+        <v>20.256</v>
+      </c>
+      <c r="K24">
+        <v>20.137499999999999</v>
+      </c>
+      <c r="L24">
+        <v>19.913499999999999</v>
+      </c>
+      <c r="M24">
+        <v>19.987500000000001</v>
+      </c>
+      <c r="N24">
+        <v>20.253</v>
+      </c>
+      <c r="O24">
+        <v>20.010999999999999</v>
+      </c>
+      <c r="P24">
+        <v>20.521999999999998</v>
+      </c>
+      <c r="Q24">
+        <v>19.925999999999998</v>
+      </c>
+      <c r="R24">
+        <v>4.9649999999999999</v>
+      </c>
+      <c r="S24">
+        <v>3.2160000000000002</v>
+      </c>
+      <c r="T24">
+        <v>3.2155999999999998</v>
+      </c>
+      <c r="U24">
+        <v>3.3051499999999998</v>
+      </c>
+      <c r="V24">
+        <v>3.2396500000000001</v>
+      </c>
+      <c r="W24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="202" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G202" t="s">
+        <v>3</v>
+      </c>
+      <c r="H202" t="s">
+        <v>4</v>
+      </c>
+      <c r="I202" t="s">
+        <v>5</v>
+      </c>
+      <c r="J202" t="s">
+        <v>6</v>
+      </c>
+      <c r="K202" t="s">
+        <v>7</v>
+      </c>
+      <c r="M202" t="s">
+        <v>44</v>
+      </c>
+      <c r="N202" t="s">
+        <v>45</v>
+      </c>
+      <c r="O202" t="s">
+        <v>46</v>
+      </c>
+      <c r="P202" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="203" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G203">
+        <v>19.322999999999997</v>
+      </c>
+      <c r="H203">
+        <v>19.092999999999996</v>
+      </c>
+      <c r="I203">
+        <v>19.421000000000006</v>
+      </c>
+      <c r="J203">
+        <v>19.536500000000004</v>
+      </c>
+      <c r="K203">
+        <v>18.442500000000003</v>
+      </c>
+      <c r="M203">
+        <v>16.997000000000003</v>
+      </c>
+      <c r="N203">
+        <v>19.322999999999997</v>
+      </c>
+      <c r="O203">
+        <v>2</v>
+      </c>
+      <c r="P203">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G204">
+        <v>17.863499999999998</v>
+      </c>
+      <c r="H204">
+        <v>17.4435</v>
+      </c>
+      <c r="I204">
+        <v>18.138999999999999</v>
+      </c>
+      <c r="J204">
+        <v>18.278999999999996</v>
+      </c>
+      <c r="K204">
+        <v>16.314500000000002</v>
+      </c>
+      <c r="M204">
+        <v>17.454499999999999</v>
+      </c>
+      <c r="N204">
+        <v>19.092999999999996</v>
+      </c>
+      <c r="O204">
+        <v>1</v>
+      </c>
+      <c r="P204">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G205">
+        <v>20.707000000000004</v>
+      </c>
+      <c r="H205">
+        <v>20.631999999999998</v>
+      </c>
+      <c r="I205">
+        <v>20.588500000000003</v>
+      </c>
+      <c r="J205">
+        <v>20.752499999999994</v>
+      </c>
+      <c r="K205">
+        <v>20.469500000000004</v>
+      </c>
+      <c r="M205">
+        <v>17.481999999999996</v>
+      </c>
+      <c r="N205">
+        <v>19.421000000000006</v>
+      </c>
+      <c r="O205">
+        <v>2</v>
+      </c>
+      <c r="P205">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M206">
+        <v>17.957000000000001</v>
+      </c>
+      <c r="N206">
+        <v>19.536500000000004</v>
+      </c>
+      <c r="O206">
+        <v>2</v>
+      </c>
+      <c r="P206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M207">
+        <v>16.222999999999999</v>
+      </c>
+      <c r="N207">
+        <v>18.442500000000003</v>
+      </c>
+      <c r="O207">
+        <v>3</v>
+      </c>
+      <c r="P207">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G208" t="s">
+        <v>8</v>
+      </c>
+      <c r="H208" t="s">
+        <v>9</v>
+      </c>
+      <c r="I208" t="s">
+        <v>11</v>
+      </c>
+      <c r="J208" t="s">
+        <v>12</v>
+      </c>
+      <c r="K208" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="209" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G209">
+        <v>16.997000000000003</v>
+      </c>
+      <c r="H209">
+        <v>17.454499999999999</v>
+      </c>
+      <c r="I209">
+        <v>17.481999999999996</v>
+      </c>
+      <c r="J209">
+        <v>17.957000000000001</v>
+      </c>
+      <c r="K209">
+        <v>16.222999999999999</v>
+      </c>
+      <c r="M209">
+        <v>11.67857143</v>
+      </c>
+      <c r="N209">
+        <v>-1.03</v>
+      </c>
+      <c r="O209">
+        <v>2</v>
+      </c>
+      <c r="P209">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G210">
+        <v>13.5785</v>
+      </c>
+      <c r="H210">
+        <v>14.568999999999999</v>
+      </c>
+      <c r="I210">
+        <v>14.564999999999998</v>
+      </c>
+      <c r="J210">
+        <v>15.456499999999997</v>
+      </c>
+      <c r="K210">
+        <v>12.2075</v>
+      </c>
+      <c r="M210">
+        <v>9.65</v>
+      </c>
+      <c r="N210">
+        <v>-0.552857143</v>
+      </c>
+      <c r="O210">
+        <v>1</v>
+      </c>
+      <c r="P210">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G211">
+        <v>20.311</v>
+      </c>
+      <c r="H211">
+        <v>20.191499999999998</v>
+      </c>
+      <c r="I211">
+        <v>20.342000000000006</v>
+      </c>
+      <c r="J211">
+        <v>20.433999999999997</v>
+      </c>
+      <c r="K211">
+        <v>20.137999999999998</v>
+      </c>
+      <c r="M211">
+        <v>7.947619048</v>
+      </c>
+      <c r="N211">
+        <v>1.6723809519999999</v>
+      </c>
+      <c r="O211">
+        <v>2</v>
+      </c>
+      <c r="P211">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M212">
+        <v>11.51142857</v>
+      </c>
+      <c r="N212">
+        <v>5.9166666670000003</v>
+      </c>
+      <c r="O212">
+        <v>2</v>
+      </c>
+      <c r="P212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M213">
+        <v>6.8490476190000003</v>
+      </c>
+      <c r="N213">
+        <v>-5.208571429</v>
+      </c>
+      <c r="O213">
+        <v>3</v>
+      </c>
+      <c r="P213">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="215" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M215">
+        <v>13.515000000000001</v>
+      </c>
+      <c r="N215">
+        <v>17.8965</v>
+      </c>
+      <c r="O215">
+        <v>2</v>
+      </c>
+      <c r="P215">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="216" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M216">
+        <v>14.098000000000001</v>
+      </c>
+      <c r="N216">
+        <v>17.334499999999998</v>
+      </c>
+      <c r="O216">
+        <v>1</v>
+      </c>
+      <c r="P216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M217">
+        <v>14.1485</v>
+      </c>
+      <c r="N217">
+        <v>17.599499999999999</v>
+      </c>
+      <c r="O217">
+        <v>2</v>
+      </c>
+      <c r="P217">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M218">
+        <v>15.339499999999999</v>
+      </c>
+      <c r="N218">
+        <v>18.086500000000001</v>
+      </c>
+      <c r="O218">
+        <v>2</v>
+      </c>
+      <c r="P218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="M219">
+        <v>12.166499999999999</v>
+      </c>
+      <c r="N219">
+        <v>16.208500000000001</v>
+      </c>
+      <c r="O219">
+        <v>3</v>
+      </c>
+      <c r="P219">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>